<commit_message>
Added macros to the template
</commit_message>
<xml_diff>
--- a/Template_Development/Template_Example.xlsx
+++ b/Template_Development/Template_Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\Template_Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3C0505-D779-4977-A344-C64C1B1FA502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56C33DF-37D3-4649-A2CC-3588B9B470D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CD82CDFE-F1ED-40B0-B6ED-832A13DC569B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CD82CDFE-F1ED-40B0-B6ED-832A13DC569B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>